<commit_message>
Changes in Scope 1 Stationary combustion code file and source data file
</commit_message>
<xml_diff>
--- a/Scope_1_stationary_fuel.xlsx
+++ b/Scope_1_stationary_fuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebs1-my.sharepoint.com/personal/ritu_stok_com/Documents/Ritu/Python Scripts/Carbon_team_Scripts/Emission_factor_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{8BD98073-4372-4DD1-A4C0-91BC7D84BA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B84E010E-5A43-4A71-9482-8F003F79EDDA}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{8BD98073-4372-4DD1-A4C0-91BC7D84BA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A389F895-A957-4340-933A-B5B179E750B3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1566BAF8-4A8D-4F98-9E32-C18EFED8963F}"/>
+    <workbookView xWindow="10656" yWindow="2424" windowWidth="17280" windowHeight="9960" xr2:uid="{1566BAF8-4A8D-4F98-9E32-C18EFED8963F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,6 +74,24 @@
     <t>Natural Gas</t>
   </si>
   <si>
+    <t>EF Country</t>
+  </si>
+  <si>
+    <t>EF Authority</t>
+  </si>
+  <si>
+    <t>EF Data Year</t>
+  </si>
+  <si>
+    <t>EF Release Year</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>US EPA Emission Factor Hub</t>
+  </si>
+  <si>
     <r>
       <t>CH</t>
     </r>
@@ -94,7 +112,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Factor (kg/ mmBtu)</t>
+      <t xml:space="preserve"> Factor (g/ mmBtu)</t>
     </r>
   </si>
   <si>
@@ -118,26 +136,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>O Factor (kg / mmBtu)</t>
-    </r>
-  </si>
-  <si>
-    <t>EF Country</t>
-  </si>
-  <si>
-    <t>EF Authority</t>
-  </si>
-  <si>
-    <t>EF Data Year</t>
-  </si>
-  <si>
-    <t>EF Release Year</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>US EPA Emission Factor Hub</t>
+      <t>O Factor (g / mmBtu)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -253,10 +253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,7 +575,7 @@
   <dimension ref="B3:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,22 +596,22 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -632,10 +628,10 @@
         <v>1E-4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4" s="3">
         <v>2021</v>
@@ -652,16 +648,16 @@
         <v>70.22</v>
       </c>
       <c r="D5" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
-        <v>5.9999999999999995E-4</v>
+        <v>0.6</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" s="3">
         <v>2021</v>
@@ -678,16 +674,16 @@
         <v>62.87</v>
       </c>
       <c r="D6" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4">
-        <v>5.9999999999999995E-4</v>
+        <v>0.6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="3">
         <v>2021</v>

</xml_diff>

<commit_message>
Changes in code for scope 1
</commit_message>
<xml_diff>
--- a/Scope_1_stationary_fuel.xlsx
+++ b/Scope_1_stationary_fuel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebs1-my.sharepoint.com/personal/ritu_stok_com/Documents/Ritu/Python Scripts/Carbon_team_Scripts/Emission_factor_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{8BD98073-4372-4DD1-A4C0-91BC7D84BA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A389F895-A957-4340-933A-B5B179E750B3}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{8BD98073-4372-4DD1-A4C0-91BC7D84BA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD78083E-BAF2-4186-B0DB-1E4175BD3BBA}"/>
   <bookViews>
-    <workbookView xWindow="10656" yWindow="2424" windowWidth="17280" windowHeight="9960" xr2:uid="{1566BAF8-4A8D-4F98-9E32-C18EFED8963F}"/>
+    <workbookView xWindow="8616" yWindow="5028" windowWidth="17280" windowHeight="9960" xr2:uid="{1566BAF8-4A8D-4F98-9E32-C18EFED8963F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="B3:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,10 +622,10 @@
         <v>53</v>
       </c>
       <c r="D4" s="4">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
-        <v>1E-4</v>
+        <v>0.1</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>9</v>

</xml_diff>